<commit_message>
fix logic bugs and modify  membershours table in database
</commit_message>
<xml_diff>
--- a/downloads/End year template.xlsx
+++ b/downloads/End year template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\Kids_uni\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF2C565-722F-46C3-A34B-7E3D5615E264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9106B821-B4E2-445D-8C16-346288DA254D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$V$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Username and passwords'!$A$6:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Username and passwords'!$A$6:$D$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -760,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V958"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:A404"/>
     </sheetView>
@@ -14807,10 +14807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:E56"/>
+  <dimension ref="A2:D56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -14819,10 +14819,9 @@
     <col min="2" max="2" width="21" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="22" customWidth="1"/>
     <col min="4" max="4" width="17.3984375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.19921875" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>32</v>
       </c>
@@ -14836,7 +14835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -14849,55 +14848,52 @@
       <c r="D6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="1:5" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
-      <c r="E56" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:E6" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E37">
+  <autoFilter ref="A6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D37">
       <sortCondition ref="A6"/>
     </sortState>
   </autoFilter>

</xml_diff>